<commit_message>
klaar zetten voor TCS versie
</commit_message>
<xml_diff>
--- a/IMKL2.x/1. dataspecificatie/IMKL-changelog dataspecificatie (Herman).xlsx
+++ b/IMKL2.x/1. dataspecificatie/IMKL-changelog dataspecificatie (Herman).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-review\IMKL2.x\1. dataspecificatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B944886-843A-4C8D-870D-3F334F914489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CBC526-C233-4E13-AA80-AD20A73C6C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Datum</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Via INSPIRE:UtilityNetwork is er met het attribuut utilityFacilityReference een referentie mogelijk naar een ActivityComplex. Hiermee kan gerefereerd worden aan grote utiliteitsnetonderdelen zoals bijvoorbeeld een energiecentrale een waterzuiveringscentrale, een overslagstation.</t>
   </si>
   <si>
-    <t>De objectklasse ActivityComplex wordt niet ondersteund door het huidige IMKL en evenmin het attribuut utilityFacilityNetwork.</t>
-  </si>
-  <si>
     <t>5.4</t>
   </si>
   <si>
@@ -569,7 +566,51 @@
     <t>direct gekoppeld</t>
   </si>
   <si>
-    <t>nog bekijken</t>
+    <t>aangepast</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">De objectklasse ActivityComplex wordt niet ondersteund door het huidige IMKL en evenmin het attribuut utilityFacilityNetwork. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>In  INSPIRE is er voor UtilityNetwork met het attribuut utilityFacilityReference een referentie mogelijk naar een ActivityComplex. Hiermee kan gerefereerd worden aan grote utiliteitsnetonderdelen zoals bijvoorbeeld een energiecentrale een waterzuiveringscentrale, een overslagstation. Het huidige IMKL ondersteunt echter niet de opname van het objecttype ActivityComplex en evenmin het attribuut utilityFacilityReference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>x maar moet nog iets genuanceerder</t>
+  </si>
+  <si>
+    <t>geen idee. Mogelijk toch beperken tot gml:LineString</t>
+  </si>
+  <si>
+    <t>x. Alleen als je daar op valideert</t>
+  </si>
+  <si>
+    <t>waarom</t>
+  </si>
+  <si>
+    <t>in GML denk ik niet. In IMKL wel</t>
+  </si>
+  <si>
+    <t>overgenomen</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1097,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1077,13 +1118,13 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1108,7 +1149,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1121,7 +1162,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1134,7 +1175,7 @@
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1154,7 +1195,7 @@
         <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1165,7 +1206,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1175,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1185,7 +1226,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -1195,10 +1236,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
@@ -1208,22 +1249,22 @@
         <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1238,7 +1279,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -1253,7 +1294,7 @@
         <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1266,7 +1307,7 @@
         <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.15">
@@ -1279,7 +1320,7 @@
         <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="24" x14ac:dyDescent="0.2">
@@ -1292,7 +1333,7 @@
         <v>27</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="36" x14ac:dyDescent="0.2">
@@ -1305,7 +1346,7 @@
         <v>29</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="132" x14ac:dyDescent="0.2">
@@ -1318,17 +1359,20 @@
         <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="63" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>55</v>
+      <c r="F22" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="31.5" x14ac:dyDescent="0.2">
@@ -1340,6 +1384,9 @@
       <c r="E23" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
@@ -1350,6 +1397,9 @@
       <c r="E24" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B25" s="5"/>
@@ -1360,8 +1410,11 @@
       <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="108" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
         <v>46</v>
@@ -1370,29 +1423,38 @@
         <v>47</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>48</v>
+        <v>70</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="E27" s="14"/>
+      <c r="F27" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="28" spans="2:6" ht="73.5" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="E28" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>60</v>
+      <c r="F28" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="36" x14ac:dyDescent="0.2">
@@ -1401,10 +1463,13 @@
         <v>36</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>57</v>
+      <c r="F29" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="31.5" x14ac:dyDescent="0.2">
@@ -1418,6 +1483,9 @@
       <c r="E30" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="2:6" ht="36" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
@@ -1429,6 +1497,9 @@
       </c>
       <c r="E31" s="6" t="s">
         <v>41</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="36" x14ac:dyDescent="0.2">
@@ -1438,86 +1509,92 @@
       <c r="E32" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="8"/>
@@ -1840,12 +1917,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072E6CDABC94C8E4D9FF787BE52A12D70" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="42d04a1539dbe8e7765031e6c6055247">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b4710195-8c97-40d8-961f-382a10a2b3ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c33fada9a9359e767f1806f1464d746a" ns2:_="">
     <xsd:import namespace="b4710195-8c97-40d8-961f-382a10a2b3ee"/>
@@ -2029,6 +2100,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
   <ds:schemaRefs>
@@ -2038,15 +2115,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C212EA7D-0640-4F31-AD84-F02D0846CE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2062,4 +2130,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>